<commit_message>
Replaced with latest version of snuggets file from another branch.
</commit_message>
<xml_diff>
--- a/disasterinfosite/data/snuggets.xlsx
+++ b/disasterinfosite/data/snuggets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eldan/Documents/github/hazardready/disaster-preparedness/disasterinfosite/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC4B6027-70CC-F841-826C-20D7D00B5911}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C488CE3-757E-7A4A-89AC-4359CC939E6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="1100" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="snuggets" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="88">
   <si>
     <t>heading</t>
   </si>
@@ -40,6 +40,9 @@
     <t>pop_alt_txt</t>
   </si>
   <si>
+    <t>pop_out_video</t>
+  </si>
+  <si>
     <t>pop_out_txt</t>
   </si>
   <si>
@@ -112,6 +115,9 @@
     <t>What's the worst that could happen</t>
   </si>
   <si>
+    <t>https://www.youtube.com/watch?v=yNN7eDXzlMo</t>
+  </si>
+  <si>
     <t>&lt;p&gt;&lt;b&gt;What does Magnitude tell us?&lt;/b&gt;&lt;br&gt;&lt;br&gt;The Richter Magnitude is a measure of how much energy is released during an earthquake. Click on the video to learn more.&lt;/p&gt;</t>
   </si>
   <si>
@@ -124,9 +130,6 @@
     <t>&lt;p&gt;&lt;b&gt;The most-likely and worst-case scenarios are one and the same. &lt;/b&gt; Seismologists (earthquake scientists) know that a magnitude 8-9 earthquake is overdue for this region. It‚Äôs not clear exactly what magnitude the earthquake will be&amp;#44; but on all accounts it is going to be big.  The shaking will last for minutes and cause light to major damage across the Northwest. Power and water could be off for days to weeks.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=yNN7eDXzlMo</t>
-  </si>
-  <si>
     <t>Be ready&amp;#44; get prepared</t>
   </si>
   <si>
@@ -139,10 +142,10 @@
     <t>&lt;p&gt; For a comprehensive list of preparedness steps check out our prepare page!&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Have a family (adults &amp; kids) communication plan &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Assemble an emergency kit (even if it‚Äôs not complete&amp;#44; every item will help)&lt;/p&gt;</t>
+    <t>&lt;p&gt;Have a family (adults &amp; kids) communication plan &lt;/p&gt;&lt;p&gt;Assemble an emergency kit (even if it's not complete, every item will help)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Assemble an emergency kit (even if it's not complete, every item will help)&lt;/p&gt;</t>
   </si>
   <si>
     <t>RDPO_counties</t>
@@ -188,6 +191,9 @@
   </si>
   <si>
     <t>Other important details for your location</t>
+  </si>
+  <si>
+    <t>https://youtu.be/4Uwxr42JqYQ</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;h4&gt;What is Liquefaction?&lt;/h4&gt;_x000D_
@@ -198,9 +204,6 @@
   </si>
   <si>
     <t>&lt;p&gt;This area is on solid rock or peat. It is not prone to liquefaction when shaken.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>https://youtu.be/4Uwxr42JqYQ</t>
   </si>
   <si>
     <t>&lt;p&gt;This area is at low risk for liquefaction. Unless shaking is strong it is unlikely you will see liquefaction here.&lt;/p&gt;</t>
@@ -1130,13 +1133,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1179,997 +1182,1000 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="I2">
-        <v>1</v>
+      <c r="I2" t="s">
+        <v>18</v>
       </c>
       <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
         <v>25</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
       </c>
       <c r="L2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3">
         <v>2</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>55</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
       </c>
       <c r="L3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
         <v>17</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4">
         <v>3</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>75</v>
-      </c>
-      <c r="K4" t="s">
-        <v>22</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
         <v>17</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5">
         <v>4</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>85</v>
-      </c>
-      <c r="K5" t="s">
-        <v>24</v>
       </c>
       <c r="L5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
         <v>17</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6">
         <v>5</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>95</v>
-      </c>
-      <c r="K6" t="s">
-        <v>26</v>
       </c>
       <c r="L6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7">
         <v>3</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>75</v>
-      </c>
-      <c r="K7" t="s">
-        <v>22</v>
       </c>
       <c r="L7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8">
         <v>4</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>85</v>
-      </c>
-      <c r="K8" t="s">
-        <v>24</v>
       </c>
       <c r="L8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I10" t="s">
-        <v>32</v>
-      </c>
-      <c r="L10" t="s">
         <v>33</v>
       </c>
-      <c r="N10" t="s">
+      <c r="J10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
         <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" t="s">
-        <v>32</v>
-      </c>
-      <c r="L12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="H13" t="s">
-        <v>31</v>
-      </c>
       <c r="I13" t="s">
-        <v>32</v>
-      </c>
-      <c r="L13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
-      <c r="H14" t="s">
-        <v>41</v>
-      </c>
       <c r="I14" t="s">
         <v>42</v>
       </c>
-      <c r="L14" t="s">
+      <c r="J14" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
-      <c r="H15" t="s">
-        <v>41</v>
-      </c>
       <c r="I15" t="s">
-        <v>44</v>
-      </c>
-      <c r="L15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="H16" t="s">
-        <v>41</v>
-      </c>
       <c r="I16" t="s">
-        <v>46</v>
-      </c>
-      <c r="L16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
-      <c r="H17" t="s">
-        <v>41</v>
-      </c>
       <c r="I17" t="s">
-        <v>48</v>
-      </c>
-      <c r="L17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
-      <c r="H18" t="s">
-        <v>41</v>
-      </c>
       <c r="I18" t="s">
-        <v>50</v>
-      </c>
-      <c r="L18" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
-      <c r="H19" t="s">
-        <v>31</v>
-      </c>
       <c r="I19" t="s">
-        <v>32</v>
-      </c>
-      <c r="L19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="J19" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20">
         <v>5</v>
       </c>
-      <c r="H20" t="s">
-        <v>31</v>
-      </c>
       <c r="I20" t="s">
-        <v>32</v>
-      </c>
-      <c r="L20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="J20" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21">
         <v>6</v>
       </c>
-      <c r="H21" t="s">
-        <v>31</v>
-      </c>
       <c r="I21" t="s">
-        <v>32</v>
-      </c>
-      <c r="L21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="J21" t="s">
+        <v>34</v>
+      </c>
+      <c r="M21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" t="s">
+        <v>59</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="M23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
         <v>56</v>
       </c>
-      <c r="H23" t="s">
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
         <v>57</v>
       </c>
-      <c r="I23">
+      <c r="H24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" t="s">
+        <v>59</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="M24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" t="s">
+        <v>59</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I26" t="s">
+        <v>59</v>
+      </c>
+      <c r="J26">
+        <v>3</v>
+      </c>
+      <c r="M26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I27" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27">
         <v>0</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="N23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1" t="s">
+      <c r="I28" t="s">
+        <v>64</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="M28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
         <v>56</v>
       </c>
-      <c r="H24" t="s">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
         <v>57</v>
       </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-      <c r="L24" t="s">
-        <v>60</v>
-      </c>
-      <c r="N24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1" t="s">
+      <c r="H29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
         <v>56</v>
       </c>
-      <c r="H25" t="s">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
         <v>57</v>
       </c>
-      <c r="I25">
-        <v>2</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1" t="s">
+      <c r="H30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I30" t="s">
+        <v>64</v>
+      </c>
+      <c r="J30">
+        <v>3</v>
+      </c>
+      <c r="M30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s">
         <v>56</v>
       </c>
-      <c r="H26" t="s">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
         <v>57</v>
       </c>
-      <c r="I26">
-        <v>3</v>
-      </c>
-      <c r="L26" t="s">
-        <v>62</v>
-      </c>
-      <c r="N26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="H31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I31" t="s">
+        <v>64</v>
+      </c>
+      <c r="J31">
+        <v>4</v>
+      </c>
+      <c r="M31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
         <v>56</v>
-      </c>
-      <c r="H27" t="s">
-        <v>63</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
-      </c>
-      <c r="L27" t="s">
-        <v>58</v>
-      </c>
-      <c r="N27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H28" t="s">
-        <v>63</v>
-      </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-      <c r="L28" t="s">
-        <v>60</v>
-      </c>
-      <c r="N28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H29" t="s">
-        <v>63</v>
-      </c>
-      <c r="I29">
-        <v>2</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="N29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H30" t="s">
-        <v>63</v>
-      </c>
-      <c r="I30">
-        <v>3</v>
-      </c>
-      <c r="L30" t="s">
-        <v>65</v>
-      </c>
-      <c r="N30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H31" t="s">
-        <v>63</v>
-      </c>
-      <c r="I31">
-        <v>4</v>
-      </c>
-      <c r="L31" t="s">
-        <v>66</v>
-      </c>
-      <c r="N31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" t="s">
-        <v>55</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
-      <c r="H32" t="s">
-        <v>41</v>
-      </c>
       <c r="I32" t="s">
         <v>42</v>
       </c>
-      <c r="L32" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J32" t="s">
+        <v>43</v>
+      </c>
+      <c r="M32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
-      <c r="H33" t="s">
-        <v>41</v>
-      </c>
       <c r="I33" t="s">
-        <v>44</v>
-      </c>
-      <c r="L33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="J33" t="s">
+        <v>45</v>
+      </c>
+      <c r="M33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
-      <c r="H34" t="s">
-        <v>41</v>
-      </c>
       <c r="I34" t="s">
-        <v>46</v>
-      </c>
-      <c r="L34" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="J34" t="s">
+        <v>47</v>
+      </c>
+      <c r="M34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
-      <c r="H35" t="s">
-        <v>41</v>
-      </c>
       <c r="I35" t="s">
-        <v>48</v>
-      </c>
-      <c r="L35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="J35" t="s">
+        <v>49</v>
+      </c>
+      <c r="M35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C36">
         <v>2</v>
       </c>
-      <c r="H36" t="s">
-        <v>41</v>
-      </c>
       <c r="I36" t="s">
-        <v>50</v>
-      </c>
-      <c r="L36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="J36" t="s">
+        <v>51</v>
+      </c>
+      <c r="M36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
-      <c r="H37" t="s">
-        <v>41</v>
-      </c>
       <c r="I37" t="s">
         <v>42</v>
       </c>
-      <c r="L37" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J37" t="s">
+        <v>43</v>
+      </c>
+      <c r="M37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C38">
         <v>3</v>
       </c>
-      <c r="H38" t="s">
-        <v>41</v>
-      </c>
       <c r="I38" t="s">
-        <v>44</v>
-      </c>
-      <c r="L38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="J38" t="s">
+        <v>45</v>
+      </c>
+      <c r="M38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C39">
         <v>3</v>
       </c>
-      <c r="H39" t="s">
-        <v>41</v>
-      </c>
       <c r="I39" t="s">
-        <v>46</v>
-      </c>
-      <c r="L39" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="J39" t="s">
+        <v>47</v>
+      </c>
+      <c r="M39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C40">
         <v>3</v>
       </c>
-      <c r="H40" t="s">
-        <v>41</v>
-      </c>
       <c r="I40" t="s">
-        <v>48</v>
-      </c>
-      <c r="L40" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="J40" t="s">
+        <v>49</v>
+      </c>
+      <c r="M40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C41">
         <v>3</v>
       </c>
-      <c r="H41" t="s">
-        <v>41</v>
-      </c>
       <c r="I41" t="s">
-        <v>50</v>
-      </c>
-      <c r="L41" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="J41" t="s">
+        <v>51</v>
+      </c>
+      <c r="M41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C42">
         <v>4</v>
       </c>
-      <c r="H42" t="s">
-        <v>31</v>
-      </c>
       <c r="I42" t="s">
-        <v>32</v>
-      </c>
-      <c r="L42" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="J42" t="s">
+        <v>34</v>
+      </c>
+      <c r="M42" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
-      <c r="H44" t="s">
-        <v>31</v>
-      </c>
       <c r="I44" t="s">
-        <v>32</v>
-      </c>
-      <c r="L44" t="s">
+        <v>33</v>
+      </c>
+      <c r="J44" t="s">
+        <v>34</v>
+      </c>
+      <c r="M44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" t="s">
-        <v>78</v>
       </c>
       <c r="C45">
         <v>2</v>
       </c>
-      <c r="H45" t="s">
-        <v>31</v>
-      </c>
       <c r="I45" t="s">
-        <v>32</v>
-      </c>
-      <c r="L45" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="J45" t="s">
+        <v>34</v>
+      </c>
+      <c r="M45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C46">
         <v>3</v>
       </c>
-      <c r="H46" t="s">
-        <v>31</v>
-      </c>
       <c r="I46" t="s">
-        <v>32</v>
-      </c>
-      <c r="L46" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="J46" t="s">
+        <v>34</v>
+      </c>
+      <c r="M46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
-      <c r="H48" t="s">
-        <v>31</v>
-      </c>
       <c r="I48" t="s">
-        <v>32</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="M48" t="s">
+        <v>33</v>
+      </c>
+      <c r="J48" t="s">
+        <v>34</v>
+      </c>
+      <c r="M48" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N48" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
-      <c r="H51" t="s">
-        <v>41</v>
-      </c>
-      <c r="L51" t="s">
-        <v>86</v>
+      <c r="I51" t="s">
+        <v>42</v>
+      </c>
+      <c r="M51" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>